<commit_message>
nuevo template para los excels y se cambiaron las versiones de los POM a RELEASE.
</commit_message>
<xml_diff>
--- a/source/configuracion/ds/template.xlsx
+++ b/source/configuracion/ds/template.xlsx
@@ -18,8 +18,8 @@
     <sheet name="Referencias" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable21" hidden="1">Table2[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable41" hidden="1">Table4[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable2" hidden="1">Table2[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable4" hidden="1">Table4[]</definedName>
     <definedName name="AGC">Objetivos!$B$2:$B$4</definedName>
     <definedName name="AGC.1">Objetivos!$L$2</definedName>
     <definedName name="AGC.2">Objetivos!$L$3:$L$4</definedName>
@@ -233,7 +233,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2-ad0318f2-ed83-49bb-801e-801e7c00393c">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable21"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable2"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -242,7 +242,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table4-4cc31b37-cd3c-4785-a1be-15f247fb1e3e">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable41"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable4"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -6011,7 +6011,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BI300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="C12" sqref="C12:C13"/>
       <selection pane="topRight" activeCell="B1" sqref="B1:C1"/>
@@ -24891,7 +24891,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="L9QMoC/cdKZ4akG6w9AUr0Zpvgt2RfjYQnyZAIDDRhcqBthMOWFWniLVgjORcNXlFDbqDkmTu5FHhWQRjVFCMg==" saltValue="nQ1W6MxsJyq3W65Ip8OG7w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="8">
     <mergeCell ref="AF3:AK3"/>
@@ -43736,12 +43736,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B820CDA07FA5B44B4F83F600FD99B6C" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0216ebc27e4f313a448b3c73f7bbcbc6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2384c6cc0088fcedbaf6edaf557defa">
     <xsd:element name="properties">
@@ -43855,6 +43849,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{519C854B-DA5E-4F2F-AEC6-59C1A61E30FB}">
   <ds:schemaRefs>
@@ -43864,21 +43864,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743D4997-851C-4501-BA80-3E703D9355C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDE0AEA0-BF11-4CAB-A051-99173BB3FE72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43892,4 +43877,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743D4997-851C-4501-BA80-3E703D9355C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
nueva version con bugs arreglados y mejoras en la performance del BUS.
</commit_message>
<xml_diff>
--- a/source/configuracion/ds/template.xlsx
+++ b/source/configuracion/ds/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpciaffone\SharePoint\Seguimiento de Proyectos GCBA - Doc\Casos de Uso\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpciaffone\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,8 +18,8 @@
     <sheet name="Referencias" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable2" hidden="1">Table2[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable4" hidden="1">Table4</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable21" hidden="1">Table2[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable41" hidden="1">Table4</definedName>
     <definedName name="AGC">Objetivos!$B$2:$B$3</definedName>
     <definedName name="AGC.Areas">Referencias!$T$2:$T$13</definedName>
     <definedName name="BCBA">Objetivos!$B$4:$B$8</definedName>
@@ -33,12 +33,12 @@
     <definedName name="MCGC.Areas">Referencias!$T$48:$T$60</definedName>
     <definedName name="MDUYTGC">Objetivos!$B$32:$B$36</definedName>
     <definedName name="MDUYTGC.Areas">Referencias!$T$61:$T$84</definedName>
-    <definedName name="MDUYTGC.IVC">Objetivos!$B$129:$B$131</definedName>
-    <definedName name="MDUYTGC.IVC.Areas">Referencias!$T$85</definedName>
-    <definedName name="MDUYTGC.SBASE">Objetivos!$B$37</definedName>
-    <definedName name="MDUYTGC.SBASE.Areas">Referencias!$T$86</definedName>
-    <definedName name="MDUYTGC.STRANS">Objetivos!$B$38</definedName>
-    <definedName name="MDUYTGC.STRANS.Areas">Referencias!$T$87:$T$94</definedName>
+    <definedName name="MDUYTGCIVC">Objetivos!$B$129:$B$131</definedName>
+    <definedName name="MDUYTGCIVC.Areas">Referencias!$T$85</definedName>
+    <definedName name="MDUYTGCSBASE">Objetivos!$B$37</definedName>
+    <definedName name="MDUYTGCSBASE.Areas">Referencias!$T$86</definedName>
+    <definedName name="MDUYTGCSTRANS">Objetivos!$B$38</definedName>
+    <definedName name="MDUYTGCSTRANS.Areas">Referencias!$T$87:$T$94</definedName>
     <definedName name="MEGC">Objetivos!$B$39:$B$42</definedName>
     <definedName name="MEGC.Areas">Referencias!$T$95:$T$117</definedName>
     <definedName name="MGOBGC">Objetivos!$B$43:$B$48</definedName>
@@ -115,7 +115,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2-ad0318f2-ed83-49bb-801e-801e7c00393c">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable2"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable21"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -124,7 +124,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table4-4cc31b37-cd3c-4785-a1be-15f247fb1e3e">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable4"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Excelimportacionproyectos.xlsxTable41"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1683,15 +1683,6 @@
     <t>SECM</t>
   </si>
   <si>
-    <t>MDUYTGC.IVC</t>
-  </si>
-  <si>
-    <t>MDUYTGC.SBASE</t>
-  </si>
-  <si>
-    <t>MDUYTGC.STRANS</t>
-  </si>
-  <si>
     <t>Subsecretaría de Demanda Ciudadana, Calidad y Cercanía</t>
   </si>
   <si>
@@ -1777,9 +1768,6 @@
   </si>
   <si>
     <t>4. Algunos campos tienen validaciones de formato y opciones válidas. Prestá atención a los mensajes que se te presenten.</t>
-  </si>
-  <si>
-    <t>1. Primero tenés que seleccionar tu Jurisdicción.</t>
   </si>
   <si>
     <t>Instituto de Vivienda de la Ciudad de Buenos Aires</t>
@@ -2291,6 +2279,18 @@
 • Todos los viajes en la Ciudad puedan ser realizados en medios de transporte público.
 • Todos los ciudadanos puedan realizar trámites públicos de calidad desde su casa o con fácil acceso.</t>
     </r>
+  </si>
+  <si>
+    <t>MDUYTGCIVC</t>
+  </si>
+  <si>
+    <t>MDUYTGCSBASE</t>
+  </si>
+  <si>
+    <t>MDUYTGCSTRANS</t>
+  </si>
+  <si>
+    <t>1. Primero tenés que seleccionar tu Jurisdicción. Si tu excel es 2007 o anterior, deberás ingresar a mano el nombre completo de la jurisdicción. Igual que como lo ves en el sistema.</t>
   </si>
 </sst>
 </file>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="3" spans="1:64" s="42" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A3" s="86" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B3" s="86"/>
       <c r="C3" s="86"/>
@@ -5629,12 +5629,12 @@
       <c r="J3" s="81"/>
       <c r="K3" s="81"/>
       <c r="L3" s="87" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="M3" s="87"/>
       <c r="N3" s="87"/>
       <c r="O3" s="85" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="P3" s="85"/>
       <c r="Q3" s="85"/>
@@ -5642,7 +5642,7 @@
       <c r="S3" s="85"/>
       <c r="T3" s="85"/>
       <c r="U3" s="88" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="V3" s="88"/>
       <c r="W3" s="88"/>
@@ -5659,7 +5659,7 @@
       <c r="AH3" s="88"/>
       <c r="AI3" s="88"/>
       <c r="AJ3" s="81" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="AK3" s="81"/>
       <c r="AL3" s="81"/>
@@ -5671,38 +5671,38 @@
     <row r="4" spans="1:64" s="45" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A4" s="51"/>
       <c r="B4" s="52" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="53" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F4" s="43"/>
       <c r="G4" s="53" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I4" s="46"/>
       <c r="J4" s="46"/>
       <c r="K4" s="46"/>
       <c r="L4" s="44"/>
       <c r="M4" s="55" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="O4" s="54" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="P4" s="54" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="Q4" s="82" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="R4" s="83"/>
       <c r="S4" s="83"/>
@@ -5711,46 +5711,46 @@
       <c r="V4" s="43"/>
       <c r="W4" s="46"/>
       <c r="X4" s="59" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="Y4" s="59" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="Z4" s="46"/>
       <c r="AA4" s="59" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AB4" s="59" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AC4" s="46"/>
       <c r="AD4" s="59" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AE4" s="59" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AF4" s="46"/>
       <c r="AG4" s="59" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AH4" s="59" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AI4" s="46"/>
       <c r="AJ4" s="56" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="AK4" s="54" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="AL4" s="46"/>
       <c r="AM4" s="46"/>
       <c r="AN4" s="57" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="AO4" s="54" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:64" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -5827,7 +5827,7 @@
         <v>16</v>
       </c>
       <c r="Y5" s="17" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="Z5" s="17" t="s">
         <v>17</v>
@@ -5836,7 +5836,7 @@
         <v>18</v>
       </c>
       <c r="AB5" s="17" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AC5" s="17" t="s">
         <v>19</v>
@@ -5845,7 +5845,7 @@
         <v>20</v>
       </c>
       <c r="AE5" s="17" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AF5" s="17" t="s">
         <v>21</v>
@@ -5854,10 +5854,10 @@
         <v>22</v>
       </c>
       <c r="AH5" s="17" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="AI5" s="17" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AJ5" s="17" t="s">
         <v>107</v>
@@ -6099,7 +6099,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6116,22 +6116,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="80" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
-        <v>548</v>
+        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6166,7 +6166,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6180,28 +6180,28 @@
     </row>
     <row r="17" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="80" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="89" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D18" s="13"/>
       <c r="F18" s="14"/>
       <c r="G18" s="90" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B19" s="74"/>
       <c r="C19" s="89"/>
       <c r="D19" s="13"/>
       <c r="E19" s="76" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="F19" s="74"/>
       <c r="G19" s="90"/>
@@ -6226,24 +6226,24 @@
     </row>
     <row r="22" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="90" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="90" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="78" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="B23" s="74"/>
       <c r="C23" s="90"/>
       <c r="D23" s="13"/>
       <c r="E23" s="77" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="F23" s="74"/>
       <c r="G23" s="90"/>
@@ -6258,7 +6258,7 @@
       <c r="G24" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+oHworXZwpPE1rZ0uwAR82FkG7h6jNt5moXjrm+oz+6jdHn9vO0w0uW5XK7BUeg6AHa8C7PABeLs4w7iUg+3rA==" saltValue="tl25VUqX8M6rsB0T1VebFA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="useewTftL+fdDjmw1emGQW8QQ+RXSa+VoBAR99KJHy6On1niNqZLq+0fjUuqvJhHKsMArYDkno/DhQVmAwJwsA==" saltValue="tYfglbVrQeie7zz6hiKGrQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="G18:G19"/>
@@ -6276,7 +6276,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6314,7 +6316,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6333,7 +6335,7 @@
         <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6352,7 +6354,7 @@
         <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6371,7 +6373,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6390,7 +6392,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6409,7 +6411,7 @@
         <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6428,7 +6430,7 @@
         <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C8" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6447,7 +6449,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6466,7 +6468,7 @@
         <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6485,7 +6487,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6504,7 +6506,7 @@
         <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6523,7 +6525,7 @@
         <v>71</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C13" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6542,7 +6544,7 @@
         <v>71</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6561,7 +6563,7 @@
         <v>71</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C15" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6582,7 +6584,7 @@
         <v>71</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6601,7 +6603,7 @@
         <v>71</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C17" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6621,7 +6623,7 @@
         <v>71</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C18" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6640,7 +6642,7 @@
         <v>71</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C19" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6660,7 +6662,7 @@
         <v>71</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C20" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6679,7 +6681,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C21" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6698,7 +6700,7 @@
         <v>72</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6720,7 +6722,7 @@
         <v>72</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="C23" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6739,7 +6741,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C24" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6758,7 +6760,7 @@
         <v>72</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C25" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6777,7 +6779,7 @@
         <v>72</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="C26" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6796,7 +6798,7 @@
         <v>72</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C27" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6891,7 +6893,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C32" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6910,7 +6912,7 @@
         <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C33" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6929,7 +6931,7 @@
         <v>73</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C34" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6948,7 +6950,7 @@
         <v>73</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C35" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6967,7 +6969,7 @@
         <v>73</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C36" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6986,7 +6988,7 @@
         <v>223</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C37" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6994,7 +6996,7 @@
       </c>
       <c r="D37" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.SBASE</v>
+        <v>MDUYTGCSBASE</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -7005,7 +7007,7 @@
         <v>225</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C38" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7013,7 +7015,7 @@
       </c>
       <c r="D38" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -7024,7 +7026,7 @@
         <v>389</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C39" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7043,7 +7045,7 @@
         <v>389</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C40" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7062,7 +7064,7 @@
         <v>389</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C41" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7081,7 +7083,7 @@
         <v>389</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C42" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7100,7 +7102,7 @@
         <v>74</v>
       </c>
       <c r="B43" s="71" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C43" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7119,7 +7121,7 @@
         <v>74</v>
       </c>
       <c r="B44" s="71" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C44" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7138,7 +7140,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="71" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C45" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7157,7 +7159,7 @@
         <v>74</v>
       </c>
       <c r="B46" s="72" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C46" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7176,7 +7178,7 @@
         <v>74</v>
       </c>
       <c r="B47" s="72" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C47" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7195,7 +7197,7 @@
         <v>74</v>
       </c>
       <c r="B48" s="72" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C48" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7214,7 +7216,7 @@
         <v>75</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C49" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7233,7 +7235,7 @@
         <v>75</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C50" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7252,7 +7254,7 @@
         <v>75</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C51" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7271,7 +7273,7 @@
         <v>75</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C52" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7290,7 +7292,7 @@
         <v>75</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C53" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7309,7 +7311,7 @@
         <v>75</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C54" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7328,7 +7330,7 @@
         <v>299</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C55" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7347,7 +7349,7 @@
         <v>299</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C56" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7366,7 +7368,7 @@
         <v>299</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C57" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7385,7 +7387,7 @@
         <v>299</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C58" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7404,7 +7406,7 @@
         <v>76</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C59" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7423,7 +7425,7 @@
         <v>76</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C60" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7442,7 +7444,7 @@
         <v>76</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C61" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7461,7 +7463,7 @@
         <v>76</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C62" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7480,7 +7482,7 @@
         <v>76</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C63" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7499,7 +7501,7 @@
         <v>76</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C64" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7518,7 +7520,7 @@
         <v>76</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C65" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7537,7 +7539,7 @@
         <v>76</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C66" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7556,7 +7558,7 @@
         <v>76</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C67" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7575,7 +7577,7 @@
         <v>76</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C68" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7594,7 +7596,7 @@
         <v>76</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C69" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7613,7 +7615,7 @@
         <v>76</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C70" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7632,7 +7634,7 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C71" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7651,7 +7653,7 @@
         <v>76</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C72" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7670,7 +7672,7 @@
         <v>76</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C73" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7689,7 +7691,7 @@
         <v>76</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C74" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7708,7 +7710,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C75" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7727,7 +7729,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C76" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7746,7 +7748,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C77" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7765,7 +7767,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C78" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7784,7 +7786,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C79" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7803,7 +7805,7 @@
         <v>76</v>
       </c>
       <c r="B80" s="40" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C80" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7822,7 +7824,7 @@
         <v>76</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C81" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7841,7 +7843,7 @@
         <v>76</v>
       </c>
       <c r="B82" s="40" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C82" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7860,7 +7862,7 @@
         <v>76</v>
       </c>
       <c r="B83" s="40" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C83" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7879,7 +7881,7 @@
         <v>76</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C84" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7898,7 +7900,7 @@
         <v>76</v>
       </c>
       <c r="B85" s="40" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C85" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7917,7 +7919,7 @@
         <v>77</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="C86" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7936,7 +7938,7 @@
         <v>77</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C87" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7955,7 +7957,7 @@
         <v>77</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C88" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7974,7 +7976,7 @@
         <v>77</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C89" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7993,7 +7995,7 @@
         <v>77</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C90" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8009,10 +8011,10 @@
     </row>
     <row r="91" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C91" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8028,10 +8030,10 @@
     </row>
     <row r="92" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C92" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8240,7 +8242,7 @@
         <v>78</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C103" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8260,7 +8262,7 @@
         <v>78</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="C104" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8280,7 +8282,7 @@
         <v>78</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C105" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8300,7 +8302,7 @@
         <v>78</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C106" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8319,7 +8321,7 @@
         <v>78</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C107" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8339,7 +8341,7 @@
         <v>83</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="C108" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8358,7 +8360,7 @@
         <v>83</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C109" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8377,7 +8379,7 @@
         <v>83</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C110" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8396,7 +8398,7 @@
         <v>83</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C111" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8472,7 +8474,7 @@
         <v>79</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C115" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8491,7 +8493,7 @@
         <v>79</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C116" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8510,7 +8512,7 @@
         <v>79</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C117" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8529,7 +8531,7 @@
         <v>79</v>
       </c>
       <c r="B118" s="40" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C118" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8548,7 +8550,7 @@
         <v>80</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C119" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8586,7 +8588,7 @@
         <v>82</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C121" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8602,10 +8604,10 @@
     </row>
     <row r="122" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C122" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8621,10 +8623,10 @@
     </row>
     <row r="123" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="C123" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8640,10 +8642,10 @@
     </row>
     <row r="124" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C124" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8659,10 +8661,10 @@
     </row>
     <row r="125" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C125" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8681,7 +8683,7 @@
         <v>476</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C126" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8700,7 +8702,7 @@
         <v>476</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C127" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8719,7 +8721,7 @@
         <v>476</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C128" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8735,10 +8737,10 @@
     </row>
     <row r="129" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C129" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8746,7 +8748,7 @@
       </c>
       <c r="D129" s="40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.IVC</v>
+        <v>MDUYTGCIVC</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -8754,10 +8756,10 @@
     </row>
     <row r="130" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C130" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8765,7 +8767,7 @@
       </c>
       <c r="D130" s="40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.IVC</v>
+        <v>MDUYTGCIVC</v>
       </c>
       <c r="E130">
         <v>2</v>
@@ -8773,10 +8775,10 @@
     </row>
     <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C131" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8784,7 +8786,7 @@
       </c>
       <c r="D131" s="40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.IVC</v>
+        <v>MDUYTGCIVC</v>
       </c>
       <c r="E131">
         <v>3</v>
@@ -8795,7 +8797,7 @@
         <v>508</v>
       </c>
       <c r="B132" s="73" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C132" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8814,7 +8816,7 @@
         <v>508</v>
       </c>
       <c r="B133" s="73" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="C133" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8833,7 +8835,7 @@
         <v>508</v>
       </c>
       <c r="B134" s="73" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C134" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8852,7 +8854,7 @@
         <v>508</v>
       </c>
       <c r="B135" s="73" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C135" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8871,7 +8873,7 @@
         <v>508</v>
       </c>
       <c r="B136" s="73" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C136" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8890,7 +8892,7 @@
         <v>508</v>
       </c>
       <c r="B137" s="73" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C137" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8905,7 +8907,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zrKyLLhdrUevgZxXUxYn2Of0d+cTmG/QelSFGmP2h7IB6ih4dDgHHrEfVnRdPivGdbm3RuxSETN7swmaLqnklQ==" saltValue="U/5Qo2/TV3AnyoUhbFhaiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="HxBNmIGIwJpwRw4lrJBbWDtq1fo/mRNHvhP6p/4sDk1MfNht7dZDWnw/gNsdyldr0k+EL8q2bNg8BXchCs4NWA==" saltValue="s4D2Zf0IrF6bKh1lNtSjRA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <tableParts count="1">
@@ -8919,9 +8921,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T372"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9238,10 +9238,10 @@
         <v>51</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>516</v>
+        <v>671</v>
       </c>
       <c r="R10" s="27" t="s">
         <v>68</v>
@@ -9265,7 +9265,7 @@
         <v>223</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>517</v>
+        <v>672</v>
       </c>
       <c r="R11" s="27" t="s">
         <v>68</v>
@@ -9289,7 +9289,7 @@
         <v>225</v>
       </c>
       <c r="P12" s="26" t="s">
-        <v>518</v>
+        <v>673</v>
       </c>
       <c r="R12" s="27" t="s">
         <v>68</v>
@@ -9451,7 +9451,7 @@
     </row>
     <row r="20" spans="15:20" x14ac:dyDescent="0.25">
       <c r="O20" s="27" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="P20" s="27" t="s">
         <v>130</v>
@@ -9667,7 +9667,7 @@
     </row>
     <row r="32" spans="15:20" x14ac:dyDescent="0.25">
       <c r="O32" s="38" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="P32" s="39" t="s">
         <v>136</v>
@@ -10633,11 +10633,11 @@
     </row>
     <row r="112" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R112" s="27" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="S112" s="31" t="str">
         <f>VLOOKUP(R112,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.IVC</v>
+        <v>MDUYTGCIVC</v>
       </c>
       <c r="T112" s="27" t="s">
         <v>234</v>
@@ -10649,7 +10649,7 @@
       </c>
       <c r="S113" s="31" t="str">
         <f>VLOOKUP(R113,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.SBASE</v>
+        <v>MDUYTGCSBASE</v>
       </c>
       <c r="T113" s="27" t="s">
         <v>224</v>
@@ -10661,7 +10661,7 @@
       </c>
       <c r="S114" s="31" t="str">
         <f>VLOOKUP(R114,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T114" s="27" t="s">
         <v>226</v>
@@ -10673,7 +10673,7 @@
       </c>
       <c r="S115" s="31" t="str">
         <f>VLOOKUP(R115,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T115" s="27" t="s">
         <v>227</v>
@@ -10685,7 +10685,7 @@
       </c>
       <c r="S116" s="31" t="str">
         <f>VLOOKUP(R116,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T116" s="27" t="s">
         <v>228</v>
@@ -10697,7 +10697,7 @@
       </c>
       <c r="S117" s="31" t="str">
         <f>VLOOKUP(R117,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T117" s="27" t="s">
         <v>229</v>
@@ -10709,7 +10709,7 @@
       </c>
       <c r="S118" s="31" t="str">
         <f>VLOOKUP(R118,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T118" s="27" t="s">
         <v>230</v>
@@ -10721,7 +10721,7 @@
       </c>
       <c r="S119" s="31" t="str">
         <f>VLOOKUP(R119,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T119" s="27" t="s">
         <v>231</v>
@@ -10733,7 +10733,7 @@
       </c>
       <c r="S120" s="31" t="str">
         <f>VLOOKUP(R120,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T120" s="27" t="s">
         <v>232</v>
@@ -10745,7 +10745,7 @@
       </c>
       <c r="S121" s="31" t="str">
         <f>VLOOKUP(R121,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC.STRANS</v>
+        <v>MDUYTGCSTRANS</v>
       </c>
       <c r="T121" s="27" t="s">
         <v>233</v>
@@ -12889,7 +12889,7 @@
     </row>
     <row r="300" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R300" s="27" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S300" s="31" t="str">
         <f>VLOOKUP(R300,Table5[#All],2,FALSE)</f>
@@ -12901,7 +12901,7 @@
     </row>
     <row r="301" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R301" s="27" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S301" s="31" t="str">
         <f>VLOOKUP(R301,Table5[#All],2,FALSE)</f>
@@ -12913,7 +12913,7 @@
     </row>
     <row r="302" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R302" s="27" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S302" s="31" t="str">
         <f>VLOOKUP(R302,Table5[#All],2,FALSE)</f>
@@ -12925,7 +12925,7 @@
     </row>
     <row r="303" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R303" s="27" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S303" s="31" t="str">
         <f>VLOOKUP(R303,Table5[#All],2,FALSE)</f>
@@ -12937,7 +12937,7 @@
     </row>
     <row r="304" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R304" s="27" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S304" s="31" t="str">
         <f>VLOOKUP(R304,Table5[#All],2,FALSE)</f>
@@ -13609,7 +13609,7 @@
     </row>
     <row r="360" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R360" s="27" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S360" s="31" t="str">
         <f>VLOOKUP(R360,Table5[#All],2,FALSE)</f>
@@ -13621,7 +13621,7 @@
     </row>
     <row r="361" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R361" s="27" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S361" s="31" t="str">
         <f>VLOOKUP(R361,Table5[#All],2,FALSE)</f>
@@ -13633,7 +13633,7 @@
     </row>
     <row r="362" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R362" s="27" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S362" s="31" t="str">
         <f>VLOOKUP(R362,Table5[#All],2,FALSE)</f>
@@ -13645,7 +13645,7 @@
     </row>
     <row r="363" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R363" s="27" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="S363" s="31" t="str">
         <f>VLOOKUP(R363,Table5[#All],2,FALSE)</f>
@@ -13764,7 +13764,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fRUet9iuAbyhLrB0x8WK098iWU08AdPqANIvlV9pJByrZ/ajQkgE+W2OBb+HaUmpbb0VD/C5l3jQ349hnIci3A==" saltValue="t+jRq987KiiRhAXV0PCArQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="k4fNNRByINC/28o7PdvysXfe6OTuZMbyTknDYOg9ZENdiN3cd0Wlo8uj1m01F7h9jmwj+SG0mXxWTM1tPinnKg==" saltValue="sgoK6wS73W074jYB1pFg/A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <sortState ref="A2:A15">
     <sortCondition ref="A1"/>
   </sortState>
@@ -13892,18 +13892,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13923,24 +13923,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743D4997-851C-4501-BA80-3E703D9355C9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{519C854B-DA5E-4F2F-AEC6-59C1A61E30FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{519C854B-DA5E-4F2F-AEC6-59C1A61E30FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743D4997-851C-4501-BA80-3E703D9355C9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
se actualizo el template de Imporacion de Proyectos.
</commit_message>
<xml_diff>
--- a/source/configuracion/ds/template.xlsx
+++ b/source/configuracion/ds/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpciaffone\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://projects.hexacta.com/SeguimientoProyectosGCBA/DocumentosFuncionales/Casos de Uso/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,12 +33,12 @@
     <definedName name="MCGC.Areas">Referencias!$T$48:$T$60</definedName>
     <definedName name="MDUYTGC">Objetivos!$B$32:$B$36</definedName>
     <definedName name="MDUYTGC.Areas">Referencias!$T$61:$T$84</definedName>
-    <definedName name="MDUYTGCIVC">Objetivos!$B$129:$B$131</definedName>
-    <definedName name="MDUYTGCIVC.Areas">Referencias!$T$85</definedName>
-    <definedName name="MDUYTGCSBASE">Objetivos!$B$37</definedName>
-    <definedName name="MDUYTGCSBASE.Areas">Referencias!$T$86</definedName>
-    <definedName name="MDUYTGCSTRANS">Objetivos!$B$38</definedName>
-    <definedName name="MDUYTGCSTRANS.Areas">Referencias!$T$87:$T$94</definedName>
+    <definedName name="MDUYTGC.IVC">Objetivos!$B$129:$B$131</definedName>
+    <definedName name="MDUYTGC.IVC.Areas">Referencias!$T$85</definedName>
+    <definedName name="MDUYTGC.SBASE">Objetivos!$B$37</definedName>
+    <definedName name="MDUYTGC.SBASE.Areas">Referencias!$T$86</definedName>
+    <definedName name="MDUYTGC.STRANS">Objetivos!$B$38</definedName>
+    <definedName name="MDUYTGC.STRANS.Areas">Referencias!$T$87:$T$94</definedName>
     <definedName name="MEGC">Objetivos!$B$39:$B$42</definedName>
     <definedName name="MEGC.Areas">Referencias!$T$95:$T$117</definedName>
     <definedName name="MGOBGC">Objetivos!$B$43:$B$48</definedName>
@@ -1683,6 +1683,15 @@
     <t>SECM</t>
   </si>
   <si>
+    <t>MDUYTGC.IVC</t>
+  </si>
+  <si>
+    <t>MDUYTGC.SBASE</t>
+  </si>
+  <si>
+    <t>MDUYTGC.STRANS</t>
+  </si>
+  <si>
     <t>Subsecretaría de Demanda Ciudadana, Calidad y Cercanía</t>
   </si>
   <si>
@@ -1768,6 +1777,9 @@
   </si>
   <si>
     <t>4. Algunos campos tienen validaciones de formato y opciones válidas. Prestá atención a los mensajes que se te presenten.</t>
+  </si>
+  <si>
+    <t>1. Primero tenés que seleccionar tu Jurisdicción.</t>
   </si>
   <si>
     <t>Instituto de Vivienda de la Ciudad de Buenos Aires</t>
@@ -2279,18 +2291,6 @@
 • Todos los viajes en la Ciudad puedan ser realizados en medios de transporte público.
 • Todos los ciudadanos puedan realizar trámites públicos de calidad desde su casa o con fácil acceso.</t>
     </r>
-  </si>
-  <si>
-    <t>MDUYTGCIVC</t>
-  </si>
-  <si>
-    <t>MDUYTGCSBASE</t>
-  </si>
-  <si>
-    <t>MDUYTGCSTRANS</t>
-  </si>
-  <si>
-    <t>1. Primero tenés que seleccionar tu Jurisdicción. Si tu excel es 2007 o anterior, deberás ingresar a mano el nombre completo de la jurisdicción. Igual que como lo ves en el sistema.</t>
   </si>
 </sst>
 </file>
@@ -5213,6 +5213,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="R1:T372" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="R1:T372"/>
+  <sortState ref="R2:T372">
+    <sortCondition ref="S1:S372"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Jurisdicción" dataDxfId="2"/>
     <tableColumn id="2" name="Cod" dataDxfId="1"/>
@@ -5614,7 +5617,7 @@
     </row>
     <row r="3" spans="1:64" s="42" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A3" s="86" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B3" s="86"/>
       <c r="C3" s="86"/>
@@ -5629,12 +5632,12 @@
       <c r="J3" s="81"/>
       <c r="K3" s="81"/>
       <c r="L3" s="87" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="M3" s="87"/>
       <c r="N3" s="87"/>
       <c r="O3" s="85" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="P3" s="85"/>
       <c r="Q3" s="85"/>
@@ -5642,7 +5645,7 @@
       <c r="S3" s="85"/>
       <c r="T3" s="85"/>
       <c r="U3" s="88" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="V3" s="88"/>
       <c r="W3" s="88"/>
@@ -5659,7 +5662,7 @@
       <c r="AH3" s="88"/>
       <c r="AI3" s="88"/>
       <c r="AJ3" s="81" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="AK3" s="81"/>
       <c r="AL3" s="81"/>
@@ -5671,38 +5674,38 @@
     <row r="4" spans="1:64" s="45" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A4" s="51"/>
       <c r="B4" s="52" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="53" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="F4" s="43"/>
       <c r="G4" s="53" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="I4" s="46"/>
       <c r="J4" s="46"/>
       <c r="K4" s="46"/>
       <c r="L4" s="44"/>
       <c r="M4" s="55" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="O4" s="54" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="P4" s="54" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="Q4" s="82" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="R4" s="83"/>
       <c r="S4" s="83"/>
@@ -5711,46 +5714,46 @@
       <c r="V4" s="43"/>
       <c r="W4" s="46"/>
       <c r="X4" s="59" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="Y4" s="59" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="Z4" s="46"/>
       <c r="AA4" s="59" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="AB4" s="59" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="AC4" s="46"/>
       <c r="AD4" s="59" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="AE4" s="59" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="AF4" s="46"/>
       <c r="AG4" s="59" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="AH4" s="59" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="AI4" s="46"/>
       <c r="AJ4" s="56" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="AK4" s="54" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="AL4" s="46"/>
       <c r="AM4" s="46"/>
       <c r="AN4" s="57" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="AO4" s="54" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:64" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -5827,7 +5830,7 @@
         <v>16</v>
       </c>
       <c r="Y5" s="17" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="Z5" s="17" t="s">
         <v>17</v>
@@ -5836,7 +5839,7 @@
         <v>18</v>
       </c>
       <c r="AB5" s="17" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="AC5" s="17" t="s">
         <v>19</v>
@@ -5845,7 +5848,7 @@
         <v>20</v>
       </c>
       <c r="AE5" s="17" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="AF5" s="17" t="s">
         <v>21</v>
@@ -5854,10 +5857,10 @@
         <v>22</v>
       </c>
       <c r="AH5" s="17" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="AI5" s="17" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="AJ5" s="17" t="s">
         <v>107</v>
@@ -6099,7 +6102,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6116,22 +6119,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="80" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
-        <v>674</v>
+        <v>548</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6166,7 +6169,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6180,28 +6183,28 @@
     </row>
     <row r="17" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="80" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="89" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="D18" s="13"/>
       <c r="F18" s="14"/>
       <c r="G18" s="90" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="B19" s="74"/>
       <c r="C19" s="89"/>
       <c r="D19" s="13"/>
       <c r="E19" s="76" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c r="F19" s="74"/>
       <c r="G19" s="90"/>
@@ -6226,24 +6229,24 @@
     </row>
     <row r="22" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="90" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="90" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="78" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
       <c r="B23" s="74"/>
       <c r="C23" s="90"/>
       <c r="D23" s="13"/>
       <c r="E23" s="77" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="F23" s="74"/>
       <c r="G23" s="90"/>
@@ -6258,7 +6261,7 @@
       <c r="G24" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="useewTftL+fdDjmw1emGQW8QQ+RXSa+VoBAR99KJHy6On1niNqZLq+0fjUuqvJhHKsMArYDkno/DhQVmAwJwsA==" saltValue="tYfglbVrQeie7zz6hiKGrQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+oHworXZwpPE1rZ0uwAR82FkG7h6jNt5moXjrm+oz+6jdHn9vO0w0uW5XK7BUeg6AHa8C7PABeLs4w7iUg+3rA==" saltValue="tl25VUqX8M6rsB0T1VebFA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="G18:G19"/>
@@ -6276,9 +6279,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6316,7 +6317,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6335,7 +6336,7 @@
         <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6354,7 +6355,7 @@
         <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6373,7 +6374,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6392,7 +6393,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6411,7 +6412,7 @@
         <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6430,7 +6431,7 @@
         <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="C8" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6449,7 +6450,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6468,7 +6469,7 @@
         <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6487,7 +6488,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6506,7 +6507,7 @@
         <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6525,7 +6526,7 @@
         <v>71</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="C13" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6544,7 +6545,7 @@
         <v>71</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6563,7 +6564,7 @@
         <v>71</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="C15" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6584,7 +6585,7 @@
         <v>71</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6603,7 +6604,7 @@
         <v>71</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="C17" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6623,7 +6624,7 @@
         <v>71</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="C18" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6642,7 +6643,7 @@
         <v>71</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="C19" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6662,7 +6663,7 @@
         <v>71</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="C20" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6681,7 +6682,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="C21" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6700,7 +6701,7 @@
         <v>72</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6722,7 +6723,7 @@
         <v>72</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="C23" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6741,7 +6742,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="C24" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6760,7 +6761,7 @@
         <v>72</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="C25" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6779,7 +6780,7 @@
         <v>72</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="C26" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6798,7 +6799,7 @@
         <v>72</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="C27" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6893,7 +6894,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="C32" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6912,7 +6913,7 @@
         <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="C33" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6931,7 +6932,7 @@
         <v>73</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="C34" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6950,7 +6951,7 @@
         <v>73</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="C35" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6969,7 +6970,7 @@
         <v>73</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="C36" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6988,7 +6989,7 @@
         <v>223</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="C37" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -6996,7 +6997,7 @@
       </c>
       <c r="D37" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSBASE</v>
+        <v>MDUYTGC.SBASE</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -7007,7 +7008,7 @@
         <v>225</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C38" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7015,7 +7016,7 @@
       </c>
       <c r="D38" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MDUYTGC.STRANS</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -7026,7 +7027,7 @@
         <v>389</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="C39" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7045,7 +7046,7 @@
         <v>389</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="C40" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7064,7 +7065,7 @@
         <v>389</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="C41" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7083,7 +7084,7 @@
         <v>389</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="C42" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7102,7 +7103,7 @@
         <v>74</v>
       </c>
       <c r="B43" s="71" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="C43" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7121,7 +7122,7 @@
         <v>74</v>
       </c>
       <c r="B44" s="71" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C44" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7140,7 +7141,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="71" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="C45" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7159,7 +7160,7 @@
         <v>74</v>
       </c>
       <c r="B46" s="72" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="C46" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7178,7 +7179,7 @@
         <v>74</v>
       </c>
       <c r="B47" s="72" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="C47" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7197,7 +7198,7 @@
         <v>74</v>
       </c>
       <c r="B48" s="72" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="C48" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7216,7 +7217,7 @@
         <v>75</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="C49" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7235,7 +7236,7 @@
         <v>75</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="C50" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7254,7 +7255,7 @@
         <v>75</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="C51" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7273,7 +7274,7 @@
         <v>75</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="C52" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7292,7 +7293,7 @@
         <v>75</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="C53" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7311,7 +7312,7 @@
         <v>75</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="C54" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7330,7 +7331,7 @@
         <v>299</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C55" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7349,7 +7350,7 @@
         <v>299</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="C56" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7368,7 +7369,7 @@
         <v>299</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="C57" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7387,7 +7388,7 @@
         <v>299</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="C58" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7406,7 +7407,7 @@
         <v>76</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="C59" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7425,7 +7426,7 @@
         <v>76</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="C60" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7444,7 +7445,7 @@
         <v>76</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="C61" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7463,7 +7464,7 @@
         <v>76</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="C62" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7482,7 +7483,7 @@
         <v>76</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="C63" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7501,7 +7502,7 @@
         <v>76</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="C64" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7520,7 +7521,7 @@
         <v>76</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="C65" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7539,7 +7540,7 @@
         <v>76</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="C66" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7558,7 +7559,7 @@
         <v>76</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="C67" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7577,7 +7578,7 @@
         <v>76</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="C68" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7596,7 +7597,7 @@
         <v>76</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="C69" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7615,7 +7616,7 @@
         <v>76</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c r="C70" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7634,7 +7635,7 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="C71" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7653,7 +7654,7 @@
         <v>76</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="C72" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7672,7 +7673,7 @@
         <v>76</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C73" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7691,7 +7692,7 @@
         <v>76</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="C74" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7710,7 +7711,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="C75" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7729,7 +7730,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="C76" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7748,7 +7749,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="C77" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7767,7 +7768,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="C78" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7786,7 +7787,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="C79" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7805,7 +7806,7 @@
         <v>76</v>
       </c>
       <c r="B80" s="40" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C80" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7824,7 +7825,7 @@
         <v>76</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="C81" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7843,7 +7844,7 @@
         <v>76</v>
       </c>
       <c r="B82" s="40" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="C82" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7862,7 +7863,7 @@
         <v>76</v>
       </c>
       <c r="B83" s="40" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="C83" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7881,7 +7882,7 @@
         <v>76</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="C84" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7900,7 +7901,7 @@
         <v>76</v>
       </c>
       <c r="B85" s="40" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="C85" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7919,7 +7920,7 @@
         <v>77</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="C86" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7938,7 +7939,7 @@
         <v>77</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="C87" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7957,7 +7958,7 @@
         <v>77</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="C88" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7976,7 +7977,7 @@
         <v>77</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="C89" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -7995,7 +7996,7 @@
         <v>77</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="C90" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8011,10 +8012,10 @@
     </row>
     <row r="91" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="C91" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8030,10 +8031,10 @@
     </row>
     <row r="92" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="C92" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8242,7 +8243,7 @@
         <v>78</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="C103" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8262,7 +8263,7 @@
         <v>78</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="C104" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8282,7 +8283,7 @@
         <v>78</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="C105" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8302,7 +8303,7 @@
         <v>78</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="C106" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8321,7 +8322,7 @@
         <v>78</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="C107" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8341,7 +8342,7 @@
         <v>83</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="C108" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8360,7 +8361,7 @@
         <v>83</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="C109" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8379,7 +8380,7 @@
         <v>83</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C110" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8398,7 +8399,7 @@
         <v>83</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="C111" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8474,7 +8475,7 @@
         <v>79</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="C115" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8493,7 +8494,7 @@
         <v>79</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="C116" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8512,7 +8513,7 @@
         <v>79</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="C117" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8531,7 +8532,7 @@
         <v>79</v>
       </c>
       <c r="B118" s="40" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="C118" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8550,7 +8551,7 @@
         <v>80</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="C119" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8588,7 +8589,7 @@
         <v>82</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="C121" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8604,10 +8605,10 @@
     </row>
     <row r="122" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="C122" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8623,10 +8624,10 @@
     </row>
     <row r="123" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="C123" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8642,10 +8643,10 @@
     </row>
     <row r="124" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="C124" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8661,10 +8662,10 @@
     </row>
     <row r="125" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="C125" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8683,7 +8684,7 @@
         <v>476</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="C126" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8702,7 +8703,7 @@
         <v>476</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="C127" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8721,7 +8722,7 @@
         <v>476</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="C128" s="3" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8737,10 +8738,10 @@
     </row>
     <row r="129" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="C129" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8748,7 +8749,7 @@
       </c>
       <c r="D129" s="40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCIVC</v>
+        <v>MDUYTGC.IVC</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -8756,10 +8757,10 @@
     </row>
     <row r="130" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="C130" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8767,7 +8768,7 @@
       </c>
       <c r="D130" s="40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCIVC</v>
+        <v>MDUYTGC.IVC</v>
       </c>
       <c r="E130">
         <v>2</v>
@@ -8775,10 +8776,10 @@
     </row>
     <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="C131" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8786,7 +8787,7 @@
       </c>
       <c r="D131" s="40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[Jurisdicción]],Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCIVC</v>
+        <v>MDUYTGC.IVC</v>
       </c>
       <c r="E131">
         <v>3</v>
@@ -8797,7 +8798,7 @@
         <v>508</v>
       </c>
       <c r="B132" s="73" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="C132" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8816,7 +8817,7 @@
         <v>508</v>
       </c>
       <c r="B133" s="73" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="C133" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8835,7 +8836,7 @@
         <v>508</v>
       </c>
       <c r="B134" s="73" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="C134" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8854,7 +8855,7 @@
         <v>508</v>
       </c>
       <c r="B135" s="73" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="C135" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8873,7 +8874,7 @@
         <v>508</v>
       </c>
       <c r="B136" s="73" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="C136" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8892,7 +8893,7 @@
         <v>508</v>
       </c>
       <c r="B137" s="73" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="C137" s="40" t="str">
         <f>LEFT(Table2[[#This Row],[Objetivo estratégico]],255)</f>
@@ -8907,7 +8908,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HxBNmIGIwJpwRw4lrJBbWDtq1fo/mRNHvhP6p/4sDk1MfNht7dZDWnw/gNsdyldr0k+EL8q2bNg8BXchCs4NWA==" saltValue="s4D2Zf0IrF6bKh1lNtSjRA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zrKyLLhdrUevgZxXUxYn2Of0d+cTmG/QelSFGmP2h7IB6ih4dDgHHrEfVnRdPivGdbm3RuxSETN7swmaLqnklQ==" saltValue="U/5Qo2/TV3AnyoUhbFhaiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <tableParts count="1">
@@ -8921,7 +8922,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T372"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9238,10 +9241,10 @@
         <v>51</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>671</v>
+        <v>516</v>
       </c>
       <c r="R10" s="27" t="s">
         <v>68</v>
@@ -9265,7 +9268,7 @@
         <v>223</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>672</v>
+        <v>517</v>
       </c>
       <c r="R11" s="27" t="s">
         <v>68</v>
@@ -9289,7 +9292,7 @@
         <v>225</v>
       </c>
       <c r="P12" s="26" t="s">
-        <v>673</v>
+        <v>518</v>
       </c>
       <c r="R12" s="27" t="s">
         <v>68</v>
@@ -9451,7 +9454,7 @@
     </row>
     <row r="20" spans="15:20" x14ac:dyDescent="0.25">
       <c r="O20" s="27" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="P20" s="27" t="s">
         <v>130</v>
@@ -9667,7 +9670,7 @@
     </row>
     <row r="32" spans="15:20" x14ac:dyDescent="0.25">
       <c r="O32" s="38" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="P32" s="39" t="s">
         <v>136</v>
@@ -10021,1214 +10024,1214 @@
     </row>
     <row r="61" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R61" s="10" t="s">
-        <v>513</v>
+        <v>73</v>
       </c>
       <c r="S61" s="31" t="str">
         <f>VLOOKUP(R61,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
-      </c>
-      <c r="T61" s="27" t="s">
-        <v>364</v>
+        <v>MDUYTGC</v>
+      </c>
+      <c r="T61" s="33" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R62" s="10" t="s">
-        <v>513</v>
+        <v>73</v>
       </c>
       <c r="S62" s="31" t="str">
         <f>VLOOKUP(R62,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
-      </c>
-      <c r="T62" s="27" t="s">
-        <v>365</v>
+        <v>MDUYTGC</v>
+      </c>
+      <c r="T62" s="33" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R63" s="10" t="s">
-        <v>513</v>
+      <c r="R63" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S63" s="31" t="str">
         <f>VLOOKUP(R63,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T63" s="27" t="s">
-        <v>366</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R64" s="10" t="s">
-        <v>513</v>
+      <c r="R64" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S64" s="31" t="str">
         <f>VLOOKUP(R64,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T64" s="27" t="s">
-        <v>367</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R65" s="10" t="s">
-        <v>513</v>
+      <c r="R65" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S65" s="31" t="str">
         <f>VLOOKUP(R65,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T65" s="27" t="s">
-        <v>368</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R66" s="10" t="s">
-        <v>513</v>
+      <c r="R66" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S66" s="31" t="str">
         <f>VLOOKUP(R66,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T66" s="27" t="s">
-        <v>369</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R67" s="10" t="s">
-        <v>513</v>
+      <c r="R67" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S67" s="31" t="str">
         <f>VLOOKUP(R67,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T67" s="27" t="s">
-        <v>370</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R68" s="10" t="s">
-        <v>513</v>
+      <c r="R68" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S68" s="31" t="str">
         <f>VLOOKUP(R68,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T68" s="27" t="s">
-        <v>371</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R69" s="10" t="s">
-        <v>513</v>
+      <c r="R69" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S69" s="31" t="str">
         <f>VLOOKUP(R69,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T69" s="27" t="s">
-        <v>372</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R70" s="10" t="s">
-        <v>513</v>
+      <c r="R70" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S70" s="31" t="str">
         <f>VLOOKUP(R70,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T70" s="27" t="s">
-        <v>373</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R71" s="10" t="s">
-        <v>513</v>
+      <c r="R71" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S71" s="31" t="str">
         <f>VLOOKUP(R71,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T71" s="27" t="s">
-        <v>374</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R72" s="10" t="s">
-        <v>513</v>
+      <c r="R72" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S72" s="31" t="str">
         <f>VLOOKUP(R72,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T72" s="27" t="s">
-        <v>375</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R73" s="10" t="s">
-        <v>513</v>
+      <c r="R73" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S73" s="31" t="str">
         <f>VLOOKUP(R73,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T73" s="27" t="s">
-        <v>376</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R74" s="10" t="s">
-        <v>513</v>
+      <c r="R74" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S74" s="31" t="str">
         <f>VLOOKUP(R74,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T74" s="27" t="s">
-        <v>377</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R75" s="10" t="s">
-        <v>513</v>
+      <c r="R75" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S75" s="31" t="str">
         <f>VLOOKUP(R75,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T75" s="27" t="s">
-        <v>378</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R76" s="10" t="s">
-        <v>513</v>
+      <c r="R76" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S76" s="31" t="str">
         <f>VLOOKUP(R76,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T76" s="27" t="s">
-        <v>379</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R77" s="10" t="s">
-        <v>513</v>
+      <c r="R77" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S77" s="31" t="str">
         <f>VLOOKUP(R77,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T77" s="27" t="s">
-        <v>380</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R78" s="10" t="s">
-        <v>513</v>
+      <c r="R78" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S78" s="31" t="str">
         <f>VLOOKUP(R78,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T78" s="27" t="s">
-        <v>381</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R79" s="10" t="s">
-        <v>513</v>
+      <c r="R79" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S79" s="31" t="str">
         <f>VLOOKUP(R79,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T79" s="27" t="s">
-        <v>382</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R80" s="10" t="s">
-        <v>513</v>
+      <c r="R80" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S80" s="31" t="str">
         <f>VLOOKUP(R80,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T80" s="27" t="s">
-        <v>383</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R81" s="10" t="s">
-        <v>513</v>
+      <c r="R81" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S81" s="31" t="str">
         <f>VLOOKUP(R81,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T81" s="27" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R82" s="10" t="s">
-        <v>513</v>
+      <c r="R82" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S82" s="31" t="str">
         <f>VLOOKUP(R82,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T82" s="27" t="s">
-        <v>384</v>
+        <v>220</v>
       </c>
     </row>
     <row r="83" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R83" s="10" t="s">
-        <v>513</v>
+      <c r="R83" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S83" s="31" t="str">
         <f>VLOOKUP(R83,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T83" s="27" t="s">
-        <v>385</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R84" s="10" t="s">
-        <v>513</v>
+      <c r="R84" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="S84" s="31" t="str">
         <f>VLOOKUP(R84,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC</v>
       </c>
       <c r="T84" s="27" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
     </row>
     <row r="85" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R85" s="10" t="s">
-        <v>513</v>
+      <c r="R85" s="27" t="s">
+        <v>549</v>
       </c>
       <c r="S85" s="31" t="str">
         <f>VLOOKUP(R85,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC.IVC</v>
       </c>
       <c r="T85" s="27" t="s">
-        <v>386</v>
+        <v>234</v>
       </c>
     </row>
     <row r="86" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R86" s="10" t="s">
-        <v>513</v>
+      <c r="R86" s="27" t="s">
+        <v>223</v>
       </c>
       <c r="S86" s="31" t="str">
         <f>VLOOKUP(R86,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC.SBASE</v>
       </c>
       <c r="T86" s="27" t="s">
-        <v>387</v>
+        <v>224</v>
       </c>
     </row>
     <row r="87" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R87" s="10" t="s">
-        <v>513</v>
+      <c r="R87" s="27" t="s">
+        <v>225</v>
       </c>
       <c r="S87" s="31" t="str">
         <f>VLOOKUP(R87,Table5[#All],2,FALSE)</f>
-        <v>MHYDHGC</v>
+        <v>MDUYTGC.STRANS</v>
       </c>
       <c r="T87" s="27" t="s">
-        <v>388</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R88" s="27" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="S88" s="31" t="str">
         <f>VLOOKUP(R88,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
-      </c>
-      <c r="T88" s="33" t="s">
-        <v>201</v>
+        <v>MDUYTGC.STRANS</v>
+      </c>
+      <c r="T88" s="27" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R89" s="32" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="S89" s="31" t="str">
         <f>VLOOKUP(R89,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
-      </c>
-      <c r="T89" s="33" t="s">
-        <v>170</v>
+        <v>MDUYTGC.STRANS</v>
+      </c>
+      <c r="T89" s="27" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R90" s="27" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="S90" s="31" t="str">
         <f>VLOOKUP(R90,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MDUYTGC.STRANS</v>
       </c>
       <c r="T90" s="27" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R91" s="27" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="S91" s="31" t="str">
         <f>VLOOKUP(R91,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MDUYTGC.STRANS</v>
       </c>
       <c r="T91" s="27" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R92" s="27" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="S92" s="31" t="str">
         <f>VLOOKUP(R92,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MDUYTGC.STRANS</v>
       </c>
       <c r="T92" s="27" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R93" s="27" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="S93" s="31" t="str">
         <f>VLOOKUP(R93,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MDUYTGC.STRANS</v>
       </c>
       <c r="T93" s="27" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R94" s="27" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="S94" s="31" t="str">
         <f>VLOOKUP(R94,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MDUYTGC.STRANS</v>
       </c>
       <c r="T94" s="27" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R95" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S95" s="31" t="str">
         <f>VLOOKUP(R95,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T95" s="27" t="s">
-        <v>207</v>
+        <v>390</v>
       </c>
     </row>
     <row r="96" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R96" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S96" s="31" t="str">
         <f>VLOOKUP(R96,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T96" s="27" t="s">
-        <v>208</v>
+        <v>391</v>
       </c>
     </row>
     <row r="97" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R97" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S97" s="31" t="str">
         <f>VLOOKUP(R97,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T97" s="27" t="s">
-        <v>209</v>
+        <v>392</v>
       </c>
     </row>
     <row r="98" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R98" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S98" s="31" t="str">
         <f>VLOOKUP(R98,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T98" s="27" t="s">
-        <v>210</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R99" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S99" s="31" t="str">
         <f>VLOOKUP(R99,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T99" s="27" t="s">
-        <v>211</v>
+        <v>394</v>
       </c>
     </row>
     <row r="100" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R100" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S100" s="31" t="str">
         <f>VLOOKUP(R100,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T100" s="27" t="s">
-        <v>212</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R101" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S101" s="31" t="str">
         <f>VLOOKUP(R101,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T101" s="27" t="s">
-        <v>213</v>
+        <v>396</v>
       </c>
     </row>
     <row r="102" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R102" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S102" s="31" t="str">
         <f>VLOOKUP(R102,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T102" s="27" t="s">
-        <v>214</v>
+        <v>397</v>
       </c>
     </row>
     <row r="103" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R103" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S103" s="31" t="str">
         <f>VLOOKUP(R103,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T103" s="27" t="s">
-        <v>215</v>
+        <v>398</v>
       </c>
     </row>
     <row r="104" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R104" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S104" s="31" t="str">
         <f>VLOOKUP(R104,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T104" s="27" t="s">
-        <v>166</v>
+        <v>399</v>
       </c>
     </row>
     <row r="105" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R105" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S105" s="31" t="str">
         <f>VLOOKUP(R105,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T105" s="27" t="s">
-        <v>216</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R106" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S106" s="31" t="str">
         <f>VLOOKUP(R106,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T106" s="27" t="s">
-        <v>217</v>
+        <v>401</v>
       </c>
     </row>
     <row r="107" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R107" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S107" s="31" t="str">
         <f>VLOOKUP(R107,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T107" s="27" t="s">
-        <v>218</v>
+        <v>402</v>
       </c>
     </row>
     <row r="108" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R108" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S108" s="31" t="str">
         <f>VLOOKUP(R108,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T108" s="27" t="s">
-        <v>219</v>
+        <v>403</v>
       </c>
     </row>
     <row r="109" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R109" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S109" s="31" t="str">
         <f>VLOOKUP(R109,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T109" s="27" t="s">
-        <v>220</v>
+        <v>404</v>
       </c>
     </row>
     <row r="110" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R110" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S110" s="31" t="str">
         <f>VLOOKUP(R110,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T110" s="27" t="s">
-        <v>221</v>
+        <v>405</v>
       </c>
     </row>
     <row r="111" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R111" s="27" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
       <c r="S111" s="31" t="str">
         <f>VLOOKUP(R111,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGC</v>
+        <v>MEGC</v>
       </c>
       <c r="T111" s="27" t="s">
-        <v>222</v>
+        <v>406</v>
       </c>
     </row>
     <row r="112" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R112" s="27" t="s">
-        <v>545</v>
+        <v>389</v>
       </c>
       <c r="S112" s="31" t="str">
         <f>VLOOKUP(R112,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCIVC</v>
+        <v>MEGC</v>
       </c>
       <c r="T112" s="27" t="s">
-        <v>234</v>
+        <v>407</v>
       </c>
     </row>
     <row r="113" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R113" s="27" t="s">
-        <v>223</v>
+        <v>389</v>
       </c>
       <c r="S113" s="31" t="str">
         <f>VLOOKUP(R113,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSBASE</v>
+        <v>MEGC</v>
       </c>
       <c r="T113" s="27" t="s">
-        <v>224</v>
+        <v>408</v>
       </c>
     </row>
     <row r="114" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R114" s="27" t="s">
-        <v>225</v>
+        <v>389</v>
       </c>
       <c r="S114" s="31" t="str">
         <f>VLOOKUP(R114,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MEGC</v>
       </c>
       <c r="T114" s="27" t="s">
-        <v>226</v>
+        <v>409</v>
       </c>
     </row>
     <row r="115" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R115" s="27" t="s">
-        <v>225</v>
+        <v>389</v>
       </c>
       <c r="S115" s="31" t="str">
         <f>VLOOKUP(R115,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MEGC</v>
       </c>
       <c r="T115" s="27" t="s">
-        <v>227</v>
+        <v>410</v>
       </c>
     </row>
     <row r="116" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R116" s="10" t="s">
-        <v>225</v>
+      <c r="R116" s="27" t="s">
+        <v>389</v>
       </c>
       <c r="S116" s="31" t="str">
         <f>VLOOKUP(R116,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MEGC</v>
       </c>
       <c r="T116" s="27" t="s">
-        <v>228</v>
+        <v>411</v>
       </c>
     </row>
     <row r="117" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R117" s="27" t="s">
-        <v>225</v>
+        <v>389</v>
       </c>
       <c r="S117" s="31" t="str">
         <f>VLOOKUP(R117,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MEGC</v>
       </c>
       <c r="T117" s="27" t="s">
-        <v>229</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R118" s="27" t="s">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="S118" s="31" t="str">
         <f>VLOOKUP(R118,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T118" s="27" t="s">
-        <v>230</v>
+        <v>421</v>
       </c>
     </row>
     <row r="119" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R119" s="27" t="s">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="S119" s="31" t="str">
         <f>VLOOKUP(R119,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T119" s="27" t="s">
-        <v>231</v>
+        <v>422</v>
       </c>
     </row>
     <row r="120" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R120" s="27" t="s">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="S120" s="31" t="str">
         <f>VLOOKUP(R120,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T120" s="27" t="s">
-        <v>232</v>
+        <v>423</v>
       </c>
     </row>
     <row r="121" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R121" s="27" t="s">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="S121" s="31" t="str">
         <f>VLOOKUP(R121,Table5[#All],2,FALSE)</f>
-        <v>MDUYTGCSTRANS</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T121" s="27" t="s">
-        <v>233</v>
+        <v>424</v>
       </c>
     </row>
     <row r="122" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R122" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S122" s="31" t="str">
         <f>VLOOKUP(R122,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T122" s="27" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
     </row>
     <row r="123" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R123" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S123" s="31" t="str">
         <f>VLOOKUP(R123,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T123" s="27" t="s">
-        <v>391</v>
+        <v>426</v>
       </c>
     </row>
     <row r="124" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R124" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S124" s="31" t="str">
         <f>VLOOKUP(R124,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T124" s="27" t="s">
-        <v>392</v>
+        <v>427</v>
       </c>
     </row>
     <row r="125" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R125" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S125" s="31" t="str">
         <f>VLOOKUP(R125,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T125" s="27" t="s">
-        <v>393</v>
+        <v>428</v>
       </c>
     </row>
     <row r="126" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R126" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S126" s="31" t="str">
         <f>VLOOKUP(R126,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T126" s="27" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
     </row>
     <row r="127" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R127" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S127" s="31" t="str">
         <f>VLOOKUP(R127,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T127" s="27" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
     </row>
     <row r="128" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R128" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S128" s="31" t="str">
         <f>VLOOKUP(R128,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T128" s="27" t="s">
-        <v>396</v>
+        <v>431</v>
       </c>
     </row>
     <row r="129" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R129" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S129" s="31" t="str">
         <f>VLOOKUP(R129,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T129" s="27" t="s">
-        <v>397</v>
+        <v>432</v>
       </c>
     </row>
     <row r="130" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R130" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S130" s="31" t="str">
         <f>VLOOKUP(R130,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T130" s="27" t="s">
-        <v>398</v>
+        <v>433</v>
       </c>
     </row>
     <row r="131" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R131" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S131" s="31" t="str">
         <f>VLOOKUP(R131,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T131" s="27" t="s">
-        <v>399</v>
+        <v>434</v>
       </c>
     </row>
     <row r="132" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R132" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S132" s="31" t="str">
         <f>VLOOKUP(R132,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T132" s="27" t="s">
-        <v>400</v>
+        <v>435</v>
       </c>
     </row>
     <row r="133" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R133" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S133" s="31" t="str">
         <f>VLOOKUP(R133,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T133" s="27" t="s">
-        <v>401</v>
+        <v>436</v>
       </c>
     </row>
     <row r="134" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R134" s="27" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="S134" s="31" t="str">
         <f>VLOOKUP(R134,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MGOBGC</v>
       </c>
       <c r="T134" s="27" t="s">
-        <v>402</v>
+        <v>170</v>
       </c>
     </row>
     <row r="135" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R135" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S135" s="31" t="str">
         <f>VLOOKUP(R135,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T135" s="27" t="s">
-        <v>403</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R136" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S136" s="31" t="str">
         <f>VLOOKUP(R136,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T136" s="27" t="s">
-        <v>404</v>
+        <v>271</v>
       </c>
     </row>
     <row r="137" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R137" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S137" s="31" t="str">
         <f>VLOOKUP(R137,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T137" s="27" t="s">
-        <v>405</v>
+        <v>272</v>
       </c>
     </row>
     <row r="138" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R138" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S138" s="31" t="str">
         <f>VLOOKUP(R138,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T138" s="27" t="s">
-        <v>406</v>
+        <v>273</v>
       </c>
     </row>
     <row r="139" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R139" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S139" s="31" t="str">
         <f>VLOOKUP(R139,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T139" s="27" t="s">
-        <v>407</v>
+        <v>274</v>
       </c>
     </row>
     <row r="140" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R140" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S140" s="31" t="str">
         <f>VLOOKUP(R140,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T140" s="27" t="s">
-        <v>408</v>
+        <v>275</v>
       </c>
     </row>
     <row r="141" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R141" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S141" s="31" t="str">
         <f>VLOOKUP(R141,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T141" s="27" t="s">
-        <v>409</v>
+        <v>276</v>
       </c>
     </row>
     <row r="142" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R142" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S142" s="31" t="str">
         <f>VLOOKUP(R142,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T142" s="27" t="s">
-        <v>410</v>
+        <v>277</v>
       </c>
     </row>
     <row r="143" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R143" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S143" s="31" t="str">
         <f>VLOOKUP(R143,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T143" s="27" t="s">
-        <v>411</v>
+        <v>278</v>
       </c>
     </row>
     <row r="144" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R144" s="27" t="s">
-        <v>389</v>
+        <v>75</v>
       </c>
       <c r="S144" s="31" t="str">
         <f>VLOOKUP(R144,Table5[#All],2,FALSE)</f>
-        <v>MEGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T144" s="27" t="s">
-        <v>170</v>
+        <v>279</v>
       </c>
     </row>
     <row r="145" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R145" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S145" s="31" t="str">
         <f>VLOOKUP(R145,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T145" s="27" t="s">
-        <v>421</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R146" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S146" s="31" t="str">
         <f>VLOOKUP(R146,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T146" s="27" t="s">
-        <v>422</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R147" s="27" t="s">
-        <v>74</v>
+      <c r="R147" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="S147" s="31" t="str">
         <f>VLOOKUP(R147,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T147" s="27" t="s">
-        <v>423</v>
+        <v>282</v>
       </c>
     </row>
     <row r="148" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R148" s="27" t="s">
-        <v>74</v>
+      <c r="R148" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="S148" s="31" t="str">
         <f>VLOOKUP(R148,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T148" s="27" t="s">
-        <v>424</v>
+        <v>283</v>
       </c>
     </row>
     <row r="149" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R149" s="27" t="s">
-        <v>74</v>
+      <c r="R149" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="S149" s="31" t="str">
         <f>VLOOKUP(R149,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T149" s="27" t="s">
-        <v>425</v>
+        <v>284</v>
       </c>
     </row>
     <row r="150" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R150" s="27" t="s">
-        <v>74</v>
+      <c r="R150" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="S150" s="31" t="str">
         <f>VLOOKUP(R150,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T150" s="27" t="s">
-        <v>426</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R151" s="27" t="s">
-        <v>74</v>
+      <c r="R151" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="S151" s="31" t="str">
         <f>VLOOKUP(R151,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T151" s="27" t="s">
-        <v>427</v>
+        <v>286</v>
       </c>
     </row>
     <row r="152" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R152" s="27" t="s">
-        <v>74</v>
+      <c r="R152" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="S152" s="31" t="str">
         <f>VLOOKUP(R152,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T152" s="27" t="s">
-        <v>428</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R153" s="27" t="s">
-        <v>74</v>
+      <c r="R153" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="S153" s="31" t="str">
         <f>VLOOKUP(R153,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T153" s="27" t="s">
-        <v>429</v>
+        <v>288</v>
       </c>
     </row>
     <row r="154" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R154" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S154" s="31" t="str">
         <f>VLOOKUP(R154,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T154" s="27" t="s">
-        <v>430</v>
+        <v>289</v>
       </c>
     </row>
     <row r="155" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R155" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S155" s="31" t="str">
         <f>VLOOKUP(R155,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T155" s="27" t="s">
-        <v>431</v>
+        <v>247</v>
       </c>
     </row>
     <row r="156" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R156" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S156" s="31" t="str">
         <f>VLOOKUP(R156,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T156" s="27" t="s">
-        <v>432</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R157" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S157" s="31" t="str">
         <f>VLOOKUP(R157,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T157" s="27" t="s">
-        <v>433</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R158" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S158" s="31" t="str">
         <f>VLOOKUP(R158,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T158" s="27" t="s">
-        <v>434</v>
+        <v>291</v>
       </c>
     </row>
     <row r="159" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R159" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S159" s="31" t="str">
         <f>VLOOKUP(R159,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T159" s="27" t="s">
-        <v>435</v>
+        <v>292</v>
       </c>
     </row>
     <row r="160" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R160" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S160" s="31" t="str">
         <f>VLOOKUP(R160,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T160" s="27" t="s">
-        <v>436</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R161" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S161" s="31" t="str">
         <f>VLOOKUP(R161,Table5[#All],2,FALSE)</f>
-        <v>MGOBGC</v>
+        <v>MHGC</v>
       </c>
       <c r="T161" s="27" t="s">
-        <v>170</v>
+        <v>294</v>
       </c>
     </row>
     <row r="162" spans="18:20" x14ac:dyDescent="0.25">
@@ -11240,7 +11243,7 @@
         <v>MHGC</v>
       </c>
       <c r="T162" s="27" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" spans="18:20" x14ac:dyDescent="0.25">
@@ -11252,7 +11255,7 @@
         <v>MHGC</v>
       </c>
       <c r="T163" s="27" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="164" spans="18:20" x14ac:dyDescent="0.25">
@@ -11264,7 +11267,7 @@
         <v>MHGC</v>
       </c>
       <c r="T164" s="27" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
     </row>
     <row r="165" spans="18:20" x14ac:dyDescent="0.25">
@@ -11276,7 +11279,7 @@
         <v>MHGC</v>
       </c>
       <c r="T165" s="27" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
     </row>
     <row r="166" spans="18:20" x14ac:dyDescent="0.25">
@@ -11288,331 +11291,331 @@
         <v>MHGC</v>
       </c>
       <c r="T166" s="27" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
     </row>
     <row r="167" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R167" s="27" t="s">
-        <v>75</v>
+      <c r="R167" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S167" s="31" t="str">
         <f>VLOOKUP(R167,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T167" s="27" t="s">
-        <v>275</v>
+        <v>364</v>
       </c>
     </row>
     <row r="168" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R168" s="27" t="s">
-        <v>75</v>
+      <c r="R168" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S168" s="31" t="str">
         <f>VLOOKUP(R168,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T168" s="27" t="s">
-        <v>276</v>
+        <v>365</v>
       </c>
     </row>
     <row r="169" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R169" s="27" t="s">
-        <v>75</v>
+      <c r="R169" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S169" s="31" t="str">
         <f>VLOOKUP(R169,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T169" s="27" t="s">
-        <v>277</v>
+        <v>366</v>
       </c>
     </row>
     <row r="170" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R170" s="27" t="s">
-        <v>75</v>
+      <c r="R170" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S170" s="31" t="str">
         <f>VLOOKUP(R170,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T170" s="27" t="s">
-        <v>278</v>
+        <v>367</v>
       </c>
     </row>
     <row r="171" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R171" s="27" t="s">
-        <v>75</v>
+      <c r="R171" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S171" s="31" t="str">
         <f>VLOOKUP(R171,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T171" s="27" t="s">
-        <v>279</v>
+        <v>368</v>
       </c>
     </row>
     <row r="172" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R172" s="27" t="s">
-        <v>75</v>
+      <c r="R172" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S172" s="31" t="str">
         <f>VLOOKUP(R172,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T172" s="27" t="s">
-        <v>280</v>
+        <v>369</v>
       </c>
     </row>
     <row r="173" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R173" s="27" t="s">
-        <v>75</v>
+      <c r="R173" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S173" s="31" t="str">
         <f>VLOOKUP(R173,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T173" s="27" t="s">
-        <v>281</v>
+        <v>370</v>
       </c>
     </row>
     <row r="174" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R174" s="10" t="s">
-        <v>75</v>
+        <v>513</v>
       </c>
       <c r="S174" s="31" t="str">
         <f>VLOOKUP(R174,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T174" s="27" t="s">
-        <v>282</v>
+        <v>371</v>
       </c>
     </row>
     <row r="175" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R175" s="10" t="s">
-        <v>75</v>
+        <v>513</v>
       </c>
       <c r="S175" s="31" t="str">
         <f>VLOOKUP(R175,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T175" s="27" t="s">
-        <v>283</v>
+        <v>372</v>
       </c>
     </row>
     <row r="176" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R176" s="10" t="s">
-        <v>75</v>
+        <v>513</v>
       </c>
       <c r="S176" s="31" t="str">
         <f>VLOOKUP(R176,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T176" s="27" t="s">
-        <v>284</v>
+        <v>373</v>
       </c>
     </row>
     <row r="177" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R177" s="10" t="s">
-        <v>75</v>
+        <v>513</v>
       </c>
       <c r="S177" s="31" t="str">
         <f>VLOOKUP(R177,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T177" s="27" t="s">
-        <v>285</v>
+        <v>374</v>
       </c>
     </row>
     <row r="178" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R178" s="10" t="s">
-        <v>75</v>
+        <v>513</v>
       </c>
       <c r="S178" s="31" t="str">
         <f>VLOOKUP(R178,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T178" s="27" t="s">
-        <v>286</v>
+        <v>375</v>
       </c>
     </row>
     <row r="179" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R179" s="10" t="s">
-        <v>75</v>
+        <v>513</v>
       </c>
       <c r="S179" s="31" t="str">
         <f>VLOOKUP(R179,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T179" s="27" t="s">
-        <v>287</v>
+        <v>376</v>
       </c>
     </row>
     <row r="180" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R180" s="10" t="s">
-        <v>75</v>
+        <v>513</v>
       </c>
       <c r="S180" s="31" t="str">
         <f>VLOOKUP(R180,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T180" s="27" t="s">
-        <v>288</v>
+        <v>377</v>
       </c>
     </row>
     <row r="181" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R181" s="27" t="s">
-        <v>75</v>
+      <c r="R181" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S181" s="31" t="str">
         <f>VLOOKUP(R181,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T181" s="27" t="s">
-        <v>289</v>
+        <v>378</v>
       </c>
     </row>
     <row r="182" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R182" s="27" t="s">
-        <v>75</v>
+      <c r="R182" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S182" s="31" t="str">
         <f>VLOOKUP(R182,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T182" s="27" t="s">
-        <v>247</v>
+        <v>379</v>
       </c>
     </row>
     <row r="183" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R183" s="27" t="s">
-        <v>75</v>
+      <c r="R183" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S183" s="31" t="str">
         <f>VLOOKUP(R183,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T183" s="27" t="s">
-        <v>170</v>
+        <v>380</v>
       </c>
     </row>
     <row r="184" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R184" s="27" t="s">
-        <v>75</v>
+      <c r="R184" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S184" s="31" t="str">
         <f>VLOOKUP(R184,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T184" s="27" t="s">
-        <v>290</v>
+        <v>381</v>
       </c>
     </row>
     <row r="185" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R185" s="27" t="s">
-        <v>75</v>
+      <c r="R185" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S185" s="31" t="str">
         <f>VLOOKUP(R185,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T185" s="27" t="s">
-        <v>291</v>
+        <v>382</v>
       </c>
     </row>
     <row r="186" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R186" s="27" t="s">
-        <v>75</v>
+      <c r="R186" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S186" s="31" t="str">
         <f>VLOOKUP(R186,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T186" s="27" t="s">
-        <v>292</v>
+        <v>383</v>
       </c>
     </row>
     <row r="187" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R187" s="27" t="s">
-        <v>75</v>
+      <c r="R187" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S187" s="31" t="str">
         <f>VLOOKUP(R187,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T187" s="27" t="s">
-        <v>293</v>
+        <v>247</v>
       </c>
     </row>
     <row r="188" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R188" s="27" t="s">
-        <v>75</v>
+      <c r="R188" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S188" s="31" t="str">
         <f>VLOOKUP(R188,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T188" s="27" t="s">
-        <v>294</v>
+        <v>384</v>
       </c>
     </row>
     <row r="189" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R189" s="27" t="s">
-        <v>75</v>
+      <c r="R189" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S189" s="31" t="str">
         <f>VLOOKUP(R189,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T189" s="27" t="s">
-        <v>295</v>
+        <v>385</v>
       </c>
     </row>
     <row r="190" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R190" s="27" t="s">
-        <v>75</v>
+      <c r="R190" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S190" s="31" t="str">
         <f>VLOOKUP(R190,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T190" s="27" t="s">
-        <v>267</v>
+        <v>170</v>
       </c>
     </row>
     <row r="191" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R191" s="27" t="s">
-        <v>75</v>
+      <c r="R191" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S191" s="31" t="str">
         <f>VLOOKUP(R191,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T191" s="27" t="s">
-        <v>296</v>
+        <v>386</v>
       </c>
     </row>
     <row r="192" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R192" s="27" t="s">
-        <v>75</v>
+      <c r="R192" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S192" s="31" t="str">
         <f>VLOOKUP(R192,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T192" s="27" t="s">
-        <v>297</v>
+        <v>387</v>
       </c>
     </row>
     <row r="193" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R193" s="27" t="s">
-        <v>75</v>
+      <c r="R193" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="S193" s="31" t="str">
         <f>VLOOKUP(R193,Table5[#All],2,FALSE)</f>
-        <v>MHGC</v>
+        <v>MHYDHGC</v>
       </c>
       <c r="T193" s="27" t="s">
-        <v>298</v>
+        <v>388</v>
       </c>
     </row>
     <row r="194" spans="18:20" x14ac:dyDescent="0.25">
@@ -12889,7 +12892,7 @@
     </row>
     <row r="300" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R300" s="27" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="S300" s="31" t="str">
         <f>VLOOKUP(R300,Table5[#All],2,FALSE)</f>
@@ -12901,7 +12904,7 @@
     </row>
     <row r="301" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R301" s="27" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="S301" s="31" t="str">
         <f>VLOOKUP(R301,Table5[#All],2,FALSE)</f>
@@ -12913,7 +12916,7 @@
     </row>
     <row r="302" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R302" s="27" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="S302" s="31" t="str">
         <f>VLOOKUP(R302,Table5[#All],2,FALSE)</f>
@@ -12925,7 +12928,7 @@
     </row>
     <row r="303" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R303" s="27" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="S303" s="31" t="str">
         <f>VLOOKUP(R303,Table5[#All],2,FALSE)</f>
@@ -12937,7 +12940,7 @@
     </row>
     <row r="304" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R304" s="27" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="S304" s="31" t="str">
         <f>VLOOKUP(R304,Table5[#All],2,FALSE)</f>
@@ -13392,15 +13395,15 @@
       </c>
     </row>
     <row r="342" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R342" s="10" t="s">
-        <v>512</v>
+      <c r="R342" s="27" t="s">
+        <v>79</v>
       </c>
       <c r="S342" s="31" t="str">
         <f>VLOOKUP(R342,Table5[#All],2,FALSE)</f>
-        <v>SGYRI</v>
+        <v>SGCBA</v>
       </c>
       <c r="T342" s="27" t="s">
-        <v>442</v>
+        <v>484</v>
       </c>
     </row>
     <row r="343" spans="18:20" x14ac:dyDescent="0.25">
@@ -13412,7 +13415,7 @@
         <v>SGYRI</v>
       </c>
       <c r="T343" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="344" spans="18:20" x14ac:dyDescent="0.25">
@@ -13424,7 +13427,7 @@
         <v>SGYRI</v>
       </c>
       <c r="T344" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="345" spans="18:20" x14ac:dyDescent="0.25">
@@ -13436,7 +13439,7 @@
         <v>SGYRI</v>
       </c>
       <c r="T345" s="27" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="346" spans="18:20" x14ac:dyDescent="0.25">
@@ -13448,7 +13451,7 @@
         <v>SGYRI</v>
       </c>
       <c r="T346" s="27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="347" spans="18:20" x14ac:dyDescent="0.25">
@@ -13460,7 +13463,7 @@
         <v>SGYRI</v>
       </c>
       <c r="T347" s="27" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="348" spans="18:20" x14ac:dyDescent="0.25">
@@ -13472,7 +13475,7 @@
         <v>SGYRI</v>
       </c>
       <c r="T348" s="27" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="349" spans="18:20" x14ac:dyDescent="0.25">
@@ -13484,19 +13487,19 @@
         <v>SGYRI</v>
       </c>
       <c r="T349" s="27" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="350" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R350" s="27" t="s">
-        <v>79</v>
+      <c r="R350" s="10" t="s">
+        <v>512</v>
       </c>
       <c r="S350" s="31" t="str">
         <f>VLOOKUP(R350,Table5[#All],2,FALSE)</f>
-        <v>SGCBA</v>
+        <v>SGYRI</v>
       </c>
       <c r="T350" s="27" t="s">
-        <v>484</v>
+        <v>449</v>
       </c>
     </row>
     <row r="351" spans="18:20" x14ac:dyDescent="0.25">
@@ -13609,7 +13612,7 @@
     </row>
     <row r="360" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R360" s="27" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="S360" s="31" t="str">
         <f>VLOOKUP(R360,Table5[#All],2,FALSE)</f>
@@ -13621,7 +13624,7 @@
     </row>
     <row r="361" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R361" s="27" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="S361" s="31" t="str">
         <f>VLOOKUP(R361,Table5[#All],2,FALSE)</f>
@@ -13633,7 +13636,7 @@
     </row>
     <row r="362" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R362" s="27" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="S362" s="31" t="str">
         <f>VLOOKUP(R362,Table5[#All],2,FALSE)</f>
@@ -13645,7 +13648,7 @@
     </row>
     <row r="363" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R363" s="27" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="S363" s="31" t="str">
         <f>VLOOKUP(R363,Table5[#All],2,FALSE)</f>
@@ -13764,7 +13767,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="k4fNNRByINC/28o7PdvysXfe6OTuZMbyTknDYOg9ZENdiN3cd0Wlo8uj1m01F7h9jmwj+SG0mXxWTM1tPinnKg==" saltValue="sgoK6wS73W074jYB1pFg/A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="56ajNmTiE0n7Si/Jc3cePCfBW+zjDGYuZLoB5axV189R5CuHyWuityZOulx6zDAVeubgJFcZxDgy6zGZoOsSsg==" saltValue="Or6w0SzM4YwuG9C+86QQFQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <sortState ref="A2:A15">
     <sortCondition ref="A1"/>
   </sortState>
@@ -13778,6 +13781,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B820CDA07FA5B44B4F83F600FD99B6C" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0216ebc27e4f313a448b3c73f7bbcbc6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2384c6cc0088fcedbaf6edaf557defa">
     <xsd:element name="properties">
@@ -13891,22 +13909,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{519C854B-DA5E-4F2F-AEC6-59C1A61E30FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743D4997-851C-4501-BA80-3E703D9355C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDE0AEA0-BF11-4CAB-A051-99173BB3FE72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13920,27 +13946,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{519C854B-DA5E-4F2F-AEC6-59C1A61E30FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{743D4997-851C-4501-BA80-3E703D9355C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>